<commit_message>
Actualizacion hasta recuperar, registrar, login clase validar datos
</commit_message>
<xml_diff>
--- a/apoyo/identificacion de tablas.xlsx
+++ b/apoyo/identificacion de tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Buelvas\Desktop\Pagina_Practica_Atleticos\apoyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0CFADE-01B2-4F70-A625-35117DD717FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A0CB22-6DF6-4A7E-A0E2-90E7C0E4FE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{3A469E97-4DBD-4820-8993-B100C15EA48C}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A469E97-4DBD-4820-8993-B100C15EA48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t xml:space="preserve">Usuario </t>
   </si>
@@ -116,6 +116,33 @@
   </si>
   <si>
     <t>ejemplo*123+</t>
+  </si>
+  <si>
+    <t>registro</t>
+  </si>
+  <si>
+    <t>Tipo_Usuario</t>
+  </si>
+  <si>
+    <t>Administrador, Jugador, Generador, Representante</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Obciones</t>
+  </si>
+  <si>
+    <t>varias</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atleticos(fuerte,regular,novato, aceson-regular, asenso-novato), Space, Unicor, Pastora, </t>
   </si>
 </sst>
 </file>
@@ -167,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -294,15 +321,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -319,12 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,6 +372,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCAB19B-D38B-4C2C-AB31-5EDFAD0F8521}">
-  <dimension ref="C8:H20"/>
+  <dimension ref="C8:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,140 +711,218 @@
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+    <row r="8" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="3:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>31938</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>